<commit_message>
updated till mfg and subset
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/CreateDataConfigTest.xlsx
+++ b/resources/ExcelsheetData/CreateDataConfigTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="createNewManufacturer" sheetId="1" r:id="rId1"/>
@@ -334,18 +334,6 @@
     <t>AutomationTestChildCat16</t>
   </si>
   <si>
-    <t>ATChildCAT1</t>
-  </si>
-  <si>
-    <t>ATChildCAT2</t>
-  </si>
-  <si>
-    <t>ATChildCAT3</t>
-  </si>
-  <si>
-    <t>ATChildCAT4</t>
-  </si>
-  <si>
     <t>UserName</t>
   </si>
   <si>
@@ -398,6 +386,18 @@
   </si>
   <si>
     <t>AutomationTestCat</t>
+  </si>
+  <si>
+    <t>AutomationTestCat1</t>
+  </si>
+  <si>
+    <t>AutomationTestCat2</t>
+  </si>
+  <si>
+    <t>AutomationTestCat3</t>
+  </si>
+  <si>
+    <t>AutomationTestCat4</t>
   </si>
 </sst>
 </file>
@@ -1327,8 +1327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:Q1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1375,7 +1375,7 @@
         <v>64</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1398,7 +1398,7 @@
         <v>66</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>67</v>
@@ -1444,7 +1444,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C1" s="22" t="s">
         <v>49</v>
@@ -1453,33 +1453,33 @@
         <v>50</v>
       </c>
       <c r="E1" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="I1" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="J1" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="K1" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="L1" s="22" t="s">
         <v>111</v>
-      </c>
-      <c r="I1" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="J1" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="K1" s="22" t="s">
-        <v>114</v>
-      </c>
-      <c r="L1" s="22" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>8</v>
@@ -1491,28 +1491,28 @@
         <v>10</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="F2" s="10" t="s">
         <v>38</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="J2" s="23" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="K2" s="10" t="s">
         <v>35</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1527,8 +1527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1538,7 +1538,7 @@
     <col min="3" max="3" width="11.5703125" style="21" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.5703125" style="21" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.85546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" style="21" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25" style="21" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.42578125" style="21" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.7109375" style="21" bestFit="1" customWidth="1"/>
@@ -1591,7 +1591,7 @@
         <v>41</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>87</v>
@@ -1620,7 +1620,7 @@
         <v>41</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>88</v>
@@ -1649,7 +1649,7 @@
         <v>41</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>89</v>
@@ -1678,7 +1678,7 @@
         <v>41</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>90</v>
@@ -1707,7 +1707,7 @@
         <v>41</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>91</v>
@@ -1736,7 +1736,7 @@
         <v>41</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>92</v>
@@ -1765,7 +1765,7 @@
         <v>41</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>93</v>
@@ -1794,7 +1794,7 @@
         <v>41</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>94</v>
@@ -1823,7 +1823,7 @@
         <v>41</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>95</v>
@@ -1852,7 +1852,7 @@
         <v>41</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>96</v>
@@ -1881,7 +1881,7 @@
         <v>41</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>97</v>
@@ -1910,7 +1910,7 @@
         <v>41</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>98</v>
@@ -1939,7 +1939,7 @@
         <v>41</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>99</v>
@@ -1968,7 +1968,7 @@
         <v>41</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>100</v>
@@ -1997,7 +1997,7 @@
         <v>41</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>101</v>
@@ -2026,7 +2026,7 @@
         <v>41</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>102</v>

</xml_diff>

<commit_message>
remove config test updated and template url added
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/CreateDataConfigTest.xlsx
+++ b/resources/ExcelsheetData/CreateDataConfigTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="createNewManufacturer" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="107">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -115,9 +115,6 @@
   </si>
   <si>
     <t>Item saved Successfully</t>
-  </si>
-  <si>
-    <t>5</t>
   </si>
   <si>
     <t>TC_ItemCategorization</t>
@@ -241,12 +238,6 @@
     <t>100010000033</t>
   </si>
   <si>
-    <t>100010000333</t>
-  </si>
-  <si>
-    <t>100010003333</t>
-  </si>
-  <si>
     <t>100010000002</t>
   </si>
   <si>
@@ -259,78 +250,6 @@
     <t>100010002222</t>
   </si>
   <si>
-    <t>100010000001</t>
-  </si>
-  <si>
-    <t>100010000011</t>
-  </si>
-  <si>
-    <t>100010000111</t>
-  </si>
-  <si>
-    <t>100010001111</t>
-  </si>
-  <si>
-    <t>100010000004</t>
-  </si>
-  <si>
-    <t>100010000044</t>
-  </si>
-  <si>
-    <t>100010000444</t>
-  </si>
-  <si>
-    <t>100010004444</t>
-  </si>
-  <si>
-    <t>AutomationTestChildCat1</t>
-  </si>
-  <si>
-    <t>AutomationTestChildCat2</t>
-  </si>
-  <si>
-    <t>AutomationTestChildCat3</t>
-  </si>
-  <si>
-    <t>AutomationTestChildCat4</t>
-  </si>
-  <si>
-    <t>AutomationTestChildCat5</t>
-  </si>
-  <si>
-    <t>AutomationTestChildCat6</t>
-  </si>
-  <si>
-    <t>AutomationTestChildCat7</t>
-  </si>
-  <si>
-    <t>AutomationTestChildCat8</t>
-  </si>
-  <si>
-    <t>AutomationTestChildCat9</t>
-  </si>
-  <si>
-    <t>AutomationTestChildCat10</t>
-  </si>
-  <si>
-    <t>AutomationTestChildCat11</t>
-  </si>
-  <si>
-    <t>AutomationTestChildCat12</t>
-  </si>
-  <si>
-    <t>AutomationTestChildCat13</t>
-  </si>
-  <si>
-    <t>AutomationTestChildCat14</t>
-  </si>
-  <si>
-    <t>AutomationTestChildCat15</t>
-  </si>
-  <si>
-    <t>AutomationTestChildCat16</t>
-  </si>
-  <si>
     <t>UserName</t>
   </si>
   <si>
@@ -394,49 +313,37 @@
     <t>AutomationTestCat3</t>
   </si>
   <si>
-    <t>AutomationTestCat4</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
     <t>8</t>
   </si>
   <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>16</t>
+    <t>createChildCategories_001</t>
+  </si>
+  <si>
+    <t>createChildCategories_002</t>
+  </si>
+  <si>
+    <t>createChildCategories_003</t>
+  </si>
+  <si>
+    <t>createChildCategories_004</t>
+  </si>
+  <si>
+    <t>createChildCategories_005</t>
+  </si>
+  <si>
+    <t>createChildCategories_006</t>
+  </si>
+  <si>
+    <t>AutomationTestC1Child</t>
+  </si>
+  <si>
+    <t>AutomationTestC2Child</t>
+  </si>
+  <si>
+    <t>AutomationTestC3Child</t>
   </si>
 </sst>
 </file>
@@ -916,7 +823,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>11</v>
@@ -990,10 +897,10 @@
         <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>17</v>
@@ -1059,7 +966,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>22</v>
@@ -1074,8 +981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1131,7 +1038,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
@@ -1143,28 +1050,28 @@
         <v>10</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="G2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>31</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1211,21 +1118,21 @@
         <v>25</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G1" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>43</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>8</v>
@@ -1237,19 +1144,19 @@
         <v>10</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>31</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1283,40 +1190,40 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="C1" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="F1" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="J1" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="L1" s="13" t="s">
         <v>56</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="105" x14ac:dyDescent="0.25">
@@ -1333,28 +1240,28 @@
         <v>10</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F2" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="G2" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="H2" s="14" t="s">
+      <c r="I2" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="L2" s="14" t="s">
         <v>59</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="J2" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="K2" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="L2" s="14" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1367,7 +1274,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1387,7 +1294,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>1</v>
@@ -1396,30 +1303,30 @@
         <v>2</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F1" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" s="13" t="s">
+      <c r="I1" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="I1" s="16" t="s">
-        <v>63</v>
-      </c>
       <c r="J1" s="13" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>8</v>
@@ -1431,22 +1338,22 @@
         <v>10</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>67</v>
-      </c>
       <c r="J2" s="22" t="s">
-        <v>31</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1483,42 +1390,42 @@
         <v>0</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>102</v>
+        <v>75</v>
       </c>
       <c r="C1" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="20" t="s">
-        <v>49</v>
-      </c>
       <c r="E1" s="20" t="s">
-        <v>103</v>
+        <v>76</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>104</v>
+        <v>77</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>105</v>
+        <v>78</v>
       </c>
       <c r="H1" s="20" t="s">
-        <v>106</v>
+        <v>79</v>
       </c>
       <c r="I1" s="20" t="s">
-        <v>107</v>
+        <v>80</v>
       </c>
       <c r="J1" s="20" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="K1" s="20" t="s">
-        <v>109</v>
+        <v>82</v>
       </c>
       <c r="L1" s="20" t="s">
-        <v>110</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>111</v>
+        <v>84</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>8</v>
@@ -1530,28 +1437,28 @@
         <v>10</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>117</v>
+        <v>90</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>112</v>
+        <v>85</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>113</v>
+        <v>86</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>115</v>
+        <v>88</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>116</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1564,15 +1471,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27" style="19" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" style="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" style="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.5703125" style="19" bestFit="1" customWidth="1"/>
@@ -1586,36 +1493,36 @@
   <sheetData>
     <row r="1" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="C1" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="D1" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="23" t="s">
-        <v>49</v>
-      </c>
       <c r="E1" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F1" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G1" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="H1" s="23" t="s">
-        <v>69</v>
-      </c>
       <c r="I1" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>64</v>
+        <v>98</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>8</v>
@@ -1627,24 +1534,24 @@
         <v>10</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>120</v>
+        <v>93</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>8</v>
@@ -1656,24 +1563,24 @@
         <v>10</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>120</v>
+        <v>93</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I3" s="24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>8</v>
@@ -1685,24 +1592,24 @@
         <v>10</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>120</v>
+        <v>94</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I4" s="24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
-        <v>126</v>
+        <v>101</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>8</v>
@@ -1714,24 +1621,24 @@
         <v>10</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>120</v>
+        <v>94</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
-        <v>31</v>
+        <v>102</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>8</v>
@@ -1743,24 +1650,24 @@
         <v>10</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I6" s="24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
-        <v>127</v>
+        <v>103</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>8</v>
@@ -1772,309 +1679,19 @@
         <v>10</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I7" s="24" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="I8" s="24" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="I9" s="24" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="H10" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="I10" s="24" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="H11" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="I11" s="24" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="H12" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="I12" s="24" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="H13" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="I13" s="24" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="H14" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="I14" s="24" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="H15" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="I15" s="24" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="24" t="s">
-        <v>136</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="H16" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="I16" s="24" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="24" t="s">
-        <v>137</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="H17" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="I17" s="24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test data add/remove modules stable
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/CreateDataConfigTest.xlsx
+++ b/resources/ExcelsheetData/CreateDataConfigTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="createNewManufacturer" sheetId="1" r:id="rId1"/>
@@ -17,12 +17,12 @@
     <sheet name="createVendor" sheetId="9" r:id="rId8"/>
     <sheet name="createChildCategories" sheetId="8" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="122211" concurrentCalc="0"/>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="97">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -178,18 +178,6 @@
   </si>
   <si>
     <t>Supplier</t>
-  </si>
-  <si>
-    <t>topBanner</t>
-  </si>
-  <si>
-    <t>rightBanner</t>
-  </si>
-  <si>
-    <t>leftBanner</t>
-  </si>
-  <si>
-    <t>bottomBanner</t>
   </si>
   <si>
     <t xml:space="preserve">SaveAs </t>
@@ -199,9 +187,6 @@
 Do Not Edit this Manually.</t>
   </si>
   <si>
-    <t>test_CMS</t>
-  </si>
-  <si>
     <t>CIMM</t>
   </si>
   <si>
@@ -217,9 +202,6 @@
     <t>1</t>
   </si>
   <si>
-    <t>100000000001</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -232,24 +214,6 @@
     <t>ChildCategory Code</t>
   </si>
   <si>
-    <t>100010000003</t>
-  </si>
-  <si>
-    <t>100010000033</t>
-  </si>
-  <si>
-    <t>100010000002</t>
-  </si>
-  <si>
-    <t>100010000022</t>
-  </si>
-  <si>
-    <t>100010000222</t>
-  </si>
-  <si>
-    <t>100010002222</t>
-  </si>
-  <si>
     <t>UserName</t>
   </si>
   <si>
@@ -328,15 +292,6 @@
     <t>createChildCategories_003</t>
   </si>
   <si>
-    <t>createChildCategories_004</t>
-  </si>
-  <si>
-    <t>createChildCategories_005</t>
-  </si>
-  <si>
-    <t>createChildCategories_006</t>
-  </si>
-  <si>
     <t>AutomationTestC1Child</t>
   </si>
   <si>
@@ -344,6 +299,21 @@
   </si>
   <si>
     <t>AutomationTestC3Child</t>
+  </si>
+  <si>
+    <t>1000000000111</t>
+  </si>
+  <si>
+    <t>1000100001111</t>
+  </si>
+  <si>
+    <t>1000100002222</t>
+  </si>
+  <si>
+    <t>1000100003333</t>
+  </si>
+  <si>
+    <t>4</t>
   </si>
 </sst>
 </file>
@@ -981,7 +951,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
@@ -1071,7 +1041,7 @@
         <v>34</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1084,8 +1054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1150,13 +1120,13 @@
         <v>40</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="H2" s="10" t="s">
         <v>44</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1166,10 +1136,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1181,14 +1151,10 @@
     <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>45</v>
       </c>
@@ -1213,20 +1179,8 @@
       <c r="H1" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="14">
         <v>1</v>
       </c>
@@ -1243,25 +1197,13 @@
         <v>40</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G2" s="14" t="s">
         <v>37</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="J2" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="K2" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="L2" s="14" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1274,7 +1216,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1309,24 +1251,24 @@
         <v>39</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="G1" s="13" t="s">
         <v>41</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>8</v>
@@ -1341,19 +1283,19 @@
         <v>40</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>64</v>
+        <v>92</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J2" s="22" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1390,7 +1332,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C1" s="20" t="s">
         <v>47</v>
@@ -1399,33 +1341,33 @@
         <v>48</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="H1" s="20" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="I1" s="20" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="J1" s="20" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="K1" s="20" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="L1" s="20" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>8</v>
@@ -1437,28 +1379,28 @@
         <v>10</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="F2" s="10" t="s">
         <v>37</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="K2" s="10" t="s">
         <v>34</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1471,10 +1413,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1511,18 +1453,18 @@
         <v>41</v>
       </c>
       <c r="G1" s="23" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="H1" s="23" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="I1" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>8</v>
@@ -1537,21 +1479,21 @@
         <v>40</v>
       </c>
       <c r="F2" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="H2" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="G2" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>69</v>
-      </c>
       <c r="I2" s="24" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>8</v>
@@ -1566,21 +1508,21 @@
         <v>40</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>70</v>
+        <v>94</v>
       </c>
       <c r="I3" s="24" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>8</v>
@@ -1595,103 +1537,16 @@
         <v>40</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="I4" s="24" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="I5" s="24" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="I6" s="24" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="I7" s="24" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
items TC_80 got completed
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/CreateDataConfigTest.xlsx
+++ b/resources/ExcelsheetData/CreateDataConfigTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="4"/>
+    <workbookView minimized="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="createNewManufacturer" sheetId="1" r:id="rId1"/>
@@ -12,17 +12,18 @@
     <sheet name="createNewSubset" sheetId="3" r:id="rId3"/>
     <sheet name="createNewItem" sheetId="4" r:id="rId4"/>
     <sheet name="itemCategorization" sheetId="5" r:id="rId5"/>
-    <sheet name="createTaxonomy" sheetId="6" r:id="rId6"/>
-    <sheet name="createCategories" sheetId="7" r:id="rId7"/>
-    <sheet name="createVendor" sheetId="9" r:id="rId8"/>
-    <sheet name="createChildCategories" sheetId="8" r:id="rId9"/>
+    <sheet name="createNewProduct" sheetId="10" r:id="rId6"/>
+    <sheet name="createTaxonomy" sheetId="6" r:id="rId7"/>
+    <sheet name="createCategories" sheetId="7" r:id="rId8"/>
+    <sheet name="createVendor" sheetId="9" r:id="rId9"/>
+    <sheet name="createChildCategories" sheetId="8" r:id="rId10"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="105">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -311,6 +312,33 @@
   </si>
   <si>
     <t>1000100003333</t>
+  </si>
+  <si>
+    <t>AutomationTestProduct</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>ProductNumber</t>
+  </si>
+  <si>
+    <t>Product SuccessMessage</t>
+  </si>
+  <si>
+    <t>TestCaseId</t>
+  </si>
+  <si>
+    <t>WelcomeMessage</t>
+  </si>
+  <si>
+    <t>12345123</t>
+  </si>
+  <si>
+    <t>createNewProduct</t>
+  </si>
+  <si>
+    <t>New Product saved successfully</t>
   </si>
 </sst>
 </file>
@@ -399,7 +427,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -431,6 +459,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -804,6 +833,150 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27" style="19" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="19"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="I2" s="24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="I3" s="24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="I4" s="24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
@@ -948,7 +1121,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
@@ -1051,8 +1224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1132,6 +1305,75 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
@@ -1208,7 +1450,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
@@ -1300,7 +1542,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
@@ -1406,148 +1648,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="27" style="19" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" style="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25" style="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" style="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="19"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="G1" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="H1" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="I1" s="23" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="I2" s="24" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="I3" s="24" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="I4" s="24" t="s">
-        <v>59</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>